<commit_message>
Update template with new infrastructure
</commit_message>
<xml_diff>
--- a/4 - language metadata/lects.xlsx
+++ b/4 - language metadata/lects.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
+    <t xml:space="preserve">Orthography</t>
+  </si>
+  <si>
     <t xml:space="preserve">abui1241-lexi</t>
   </si>
   <si>
@@ -71,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">abz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p/general</t>
   </si>
 </sst>
 </file>
@@ -167,25 +173,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.35714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="60.4744897959184"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.67857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.45918367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="98.4540816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.19897959183674"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="20.6989795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -222,16 +228,19 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>-8.226</v>
@@ -240,13 +249,16 @@
         <v>124.6683</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>